<commit_message>
Update Upload File, UserShift
</commit_message>
<xml_diff>
--- a/CheckIn_Test.xlsx
+++ b/CheckIn_Test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUMMER23\SWP391\Ministore_Sonne2\MiniStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14850" windowHeight="11955"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14850" windowHeight="11960"/>
   </bookViews>
   <sheets>
     <sheet name="CheckIn" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
@@ -286,15 +286,15 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>8</v>
       </c>
@@ -302,7 +302,7 @@
         <v>45104.25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>6</v>
       </c>
@@ -310,7 +310,7 @@
         <v>45104.256944444445</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -318,7 +318,7 @@
         <v>45104.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -326,7 +326,7 @@
         <v>45104.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>6</v>
       </c>
@@ -334,7 +334,7 @@
         <v>45104.520833333336</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>7</v>
       </c>
@@ -342,15 +342,15 @@
         <v>45104.75</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="2">
-        <v>45104.753472222219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45104.770833333336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -358,7 +358,7 @@
         <v>45106.25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -366,7 +366,7 @@
         <v>45106.25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -374,7 +374,7 @@
         <v>45106.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -382,7 +382,7 @@
         <v>45106.5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -390,7 +390,7 @@
         <v>45106.510416666664</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>5</v>
       </c>
@@ -398,7 +398,7 @@
         <v>45106.75</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>3</v>
       </c>

</xml_diff>